<commit_message>
motivo: porcao cadastrado duas vezes na planilha de prazos.json
</commit_message>
<xml_diff>
--- a/data/estoque_.xlsx
+++ b/data/estoque_.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>PRODUTO</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>ANCHO MONTANA STEAKHOUSE</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>ASSADO DE TIRAS ARG</t>
@@ -255,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="16" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -281,13 +278,10 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -610,14 +604,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="52.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="13" width="10.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="15" width="25.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="15" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="11" width="52.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="14" width="25.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="14" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -674,9 +668,7 @@
       <c r="C4" s="7">
         <v>5</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
@@ -684,7 +676,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="6">
         <v>0.668</v>
@@ -700,7 +692,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="7">
         <v>6</v>
@@ -716,7 +708,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
@@ -732,7 +724,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="7">
         <v>23</v>
@@ -748,7 +740,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="6">
         <v>8.45</v>
@@ -764,7 +756,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="7">
         <v>2</v>
@@ -780,7 +772,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="7">
         <v>5</v>
@@ -796,7 +788,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="7">
         <v>4</v>
@@ -812,7 +804,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="6">
         <v>1.01</v>
@@ -828,7 +820,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="7">
         <v>0</v>
@@ -844,7 +836,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="7">
         <v>0</v>
@@ -860,7 +852,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="6">
         <v>12.37</v>
@@ -868,19 +860,15 @@
       <c r="C16" s="7">
         <v>9</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="7">
         <v>5</v>
@@ -896,7 +884,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="7">
         <v>16</v>
@@ -912,7 +900,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="7">
         <v>3</v>
@@ -928,7 +916,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="6">
         <f>21*0.3</f>
@@ -936,19 +924,15 @@
       <c r="C20" s="7">
         <v>21</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6">
         <f>21*0.5</f>
@@ -964,7 +948,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="7">
         <v>1</v>
@@ -972,9 +956,7 @@
       <c r="C22" s="7">
         <v>2</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -982,7 +964,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="7">
         <v>4</v>
@@ -990,9 +972,7 @@
       <c r="C23" s="7">
         <v>8</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1000,7 +980,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="6">
         <f>7*0.5</f>
@@ -1008,9 +988,7 @@
       <c r="C24" s="7">
         <v>7</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1018,7 +996,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="6">
         <v>4.5</v>
@@ -1026,9 +1004,7 @@
       <c r="C25" s="7">
         <v>9</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1036,7 +1012,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="6">
         <v>2.5</v>
@@ -1052,7 +1028,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
       <c r="A27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="6">
         <v>1.41</v>
@@ -1068,7 +1044,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
       <c r="A28" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="6">
         <v>0.5</v>
@@ -1076,9 +1052,7 @@
       <c r="C28" s="7">
         <v>1</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
@@ -1086,7 +1060,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
       <c r="A29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="7">
         <v>10</v>
@@ -1094,9 +1068,7 @@
       <c r="C29" s="7">
         <v>10</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -1104,7 +1076,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
       <c r="A30" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="7">
         <v>3</v>
@@ -1120,7 +1092,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
       <c r="A31" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="7">
         <v>3</v>
@@ -1136,7 +1108,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
       <c r="A32" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="7">
         <v>0</v>
@@ -1152,7 +1124,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
       <c r="A33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" s="7">
         <v>0</v>
@@ -1160,9 +1132,7 @@
       <c r="C33" s="7">
         <v>0</v>
       </c>
-      <c r="D33" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -1170,7 +1140,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
       <c r="A34" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" s="7">
         <v>1</v>
@@ -1178,17 +1148,15 @@
       <c r="C34" s="7">
         <v>1</v>
       </c>
-      <c r="D34" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="10" t="s">
-        <v>34</v>
+      <c r="A35" s="9" t="s">
+        <v>33</v>
       </c>
       <c r="B35" s="7">
         <v>2</v>
@@ -1203,8 +1171,8 @@
       <c r="H35" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="10" t="s">
-        <v>35</v>
+      <c r="A36" s="9" t="s">
+        <v>34</v>
       </c>
       <c r="B36" s="7">
         <v>4</v>
@@ -1220,7 +1188,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
       <c r="A37" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" s="6">
         <f>3.6+1.178</f>
@@ -1236,7 +1204,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="6">
         <v>1.098</v>
@@ -1251,8 +1219,8 @@
       <c r="H38" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="11" t="s">
-        <v>38</v>
+      <c r="A39" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="B39" s="6">
         <v>2.94</v>
@@ -1260,19 +1228,15 @@
       <c r="C39" s="7">
         <v>4</v>
       </c>
-      <c r="D39" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" s="6">
         <v>4.544</v>
@@ -1288,7 +1252,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" s="6">
         <v>1.55</v>
@@ -1303,8 +1267,8 @@
       <c r="H41" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
-      <c r="A42" s="11" t="s">
-        <v>41</v>
+      <c r="A42" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="B42" s="7">
         <v>0</v>
@@ -1312,19 +1276,15 @@
       <c r="C42" s="7">
         <v>0</v>
       </c>
-      <c r="D42" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E42" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="6">
         <v>1.14</v>
@@ -1340,7 +1300,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="7">
         <v>5</v>
@@ -1356,7 +1316,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="7">
         <v>4</v>
@@ -1372,7 +1332,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="6">
         <v>4.784</v>
@@ -1388,7 +1348,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" s="7">
         <v>0</v>
@@ -1404,7 +1364,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1416,7 +1376,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" s="7">
         <v>0</v>
@@ -1432,7 +1392,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" s="6">
         <v>6.5</v>
@@ -1448,7 +1408,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" s="7">
         <v>0</v>
@@ -1464,7 +1424,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" s="6">
         <v>1.05</v>
@@ -1480,7 +1440,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="7">
         <f>26*0.5</f>

</xml_diff>